<commit_message>
Extract Function Memo update
</commit_message>
<xml_diff>
--- a/doc/Notes.xlsx
+++ b/doc/Notes.xlsx
@@ -27,13 +27,13 @@
     <t>个人理解</t>
   </si>
   <si>
-    <t>把不同的逻辑抽出一个方法</t>
-  </si>
-  <si>
     <t xml:space="preserve">提炼函数（106）Extract Function </t>
   </si>
   <si>
     <t>查询取代临时变量（178）Replace Temp with Query</t>
+  </si>
+  <si>
+    <t>提炼的关键就在于命名</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,15 +416,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>